<commit_message>
Ignored and untracked files cleanup
</commit_message>
<xml_diff>
--- a/pages/ftp/RMS Aging Upload template 03.31.25.xlsx
+++ b/pages/ftp/RMS Aging Upload template 03.31.25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LNT-FIN-001\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tanholdings-my.sharepoint.com/personal/rosalie_mangulabnan_tanholdings_com/Documents/Documents/Backup folder/Drive C 2025/LNT/RMS Aging Upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E631B44B-C130-4D7D-9010-0B01986F3A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{ECF41B59-47D3-4DD0-8D79-B40AC3ED6B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E41B673F-89EC-495E-BDC1-43EF814931D4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="RMS AGING" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'RMS AGING'!$A$3:$D$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'RMS AGING'!$A$3:$D$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="149">
   <si>
     <t>Current</t>
   </si>
@@ -260,12 +260,6 @@
     <t>VELASCO, AARON A.</t>
   </si>
   <si>
-    <t>BAGUINO, GILBERT</t>
-  </si>
-  <si>
-    <t>JPC 309</t>
-  </si>
-  <si>
     <t>FT D102</t>
   </si>
   <si>
@@ -320,12 +314,6 @@
     <t>FT A207</t>
   </si>
   <si>
-    <t>NABETINAN, AGNES</t>
-  </si>
-  <si>
-    <t>FT A202</t>
-  </si>
-  <si>
     <t>April 23</t>
   </si>
   <si>
@@ -362,12 +350,6 @@
     <t>July - Nov 24</t>
   </si>
   <si>
-    <t>VILLAROSA, JOSELITO H</t>
-  </si>
-  <si>
-    <t>GC A211</t>
-  </si>
-  <si>
     <t>MABAET, CERNAN &amp;/OR MABAET, CANDIDA</t>
   </si>
   <si>
@@ -381,12 +363,6 @@
   </si>
   <si>
     <t>April - May 24</t>
-  </si>
-  <si>
-    <t>LUMBANA, CHERRY</t>
-  </si>
-  <si>
-    <t>FT B207</t>
   </si>
   <si>
     <t>POLK, JIMMY</t>
@@ -681,10 +657,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -950,12 +922,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1069,7 +1041,7 @@
         <v>153</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O4" s="8">
         <v>1</v>
@@ -1077,22 +1049,22 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
-        <v>1413826</v>
+        <v>1418448</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4">
-        <v>505</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4">
-        <v>505</v>
+        <v>25</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O5" s="8">
         <v>1</v>
@@ -1100,22 +1072,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
-        <v>1418448</v>
+        <v>1418276</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D6" s="4">
-        <v>25</v>
+        <v>352.5</v>
       </c>
       <c r="E6" s="4">
-        <v>25</v>
+        <v>352.5</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O6" s="8">
         <v>1</v>
@@ -1123,45 +1095,54 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>1418376</v>
+        <v>1418264</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="D7" s="4">
-        <v>505</v>
-      </c>
-      <c r="E7" s="4">
-        <v>505</v>
+        <v>852.83</v>
+      </c>
+      <c r="F7" s="4">
+        <v>852.83</v>
+      </c>
+      <c r="H7" s="4">
+        <v>147.83000000000001</v>
+      </c>
+      <c r="I7" s="4">
+        <v>352.5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>352.5</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="O7" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
-        <v>1418276</v>
+        <v>1418455</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D8" s="4">
-        <v>352.5</v>
+        <v>294.92</v>
       </c>
       <c r="E8" s="4">
-        <v>352.5</v>
+        <v>294.92</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O8" s="8">
         <v>1</v>
@@ -1169,31 +1150,37 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
-        <v>1418264</v>
+        <v>1416702</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4">
-        <v>852.83</v>
+        <v>2446</v>
+      </c>
+      <c r="E9" s="4">
+        <v>433</v>
       </c>
       <c r="F9" s="4">
-        <v>852.83</v>
+        <v>2013</v>
+      </c>
+      <c r="G9" s="4">
+        <v>433</v>
       </c>
       <c r="H9" s="4">
-        <v>147.83000000000001</v>
+        <v>433</v>
       </c>
       <c r="I9" s="4">
-        <v>352.5</v>
+        <v>714</v>
       </c>
       <c r="J9" s="4">
-        <v>352.5</v>
+        <v>433</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="O9" s="8">
         <v>2</v>
@@ -1201,60 +1188,54 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
-        <v>1418455</v>
+        <v>1417892</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>118</v>
+        <v>50</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
       <c r="D10" s="4">
-        <v>294.92</v>
-      </c>
-      <c r="E10" s="4">
-        <v>294.92</v>
+        <v>1057.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1057.5</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1057.5</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="O10" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
-        <v>1416702</v>
+        <v>1418163</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4">
-        <v>2446</v>
+        <v>525</v>
       </c>
       <c r="E11" s="4">
-        <v>433</v>
+        <v>505</v>
       </c>
       <c r="F11" s="4">
-        <v>2013</v>
+        <v>20</v>
       </c>
       <c r="G11" s="4">
-        <v>433</v>
-      </c>
-      <c r="H11" s="4">
-        <v>433</v>
-      </c>
-      <c r="I11" s="4">
-        <v>714</v>
-      </c>
-      <c r="J11" s="4">
-        <v>433</v>
+        <v>20</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O11" s="8">
         <v>2</v>
@@ -1262,25 +1243,28 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
-        <v>1417892</v>
+        <v>1416593</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4">
-        <v>1057.5</v>
+        <v>832</v>
+      </c>
+      <c r="E12" s="4">
+        <v>518</v>
       </c>
       <c r="F12" s="4">
-        <v>1057.5</v>
-      </c>
-      <c r="L12" s="4">
-        <v>1057.5</v>
+        <v>314</v>
+      </c>
+      <c r="G12" s="4">
+        <v>314</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="O12" s="8">
         <v>2</v>
@@ -1288,28 +1272,25 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
-        <v>1418163</v>
+        <v>1418136</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="D13" s="4">
-        <v>525</v>
-      </c>
-      <c r="E13" s="4">
         <v>505</v>
       </c>
       <c r="F13" s="4">
-        <v>20</v>
-      </c>
-      <c r="G13" s="4">
-        <v>20</v>
+        <v>505</v>
+      </c>
+      <c r="L13" s="4">
+        <v>505</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="O13" s="8">
         <v>2</v>
@@ -1317,54 +1298,48 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
-        <v>1416593</v>
+        <v>1418424</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="D14" s="4">
-        <v>832</v>
+        <v>505</v>
       </c>
       <c r="E14" s="4">
-        <v>518</v>
-      </c>
-      <c r="F14" s="4">
-        <v>314</v>
-      </c>
-      <c r="G14" s="4">
-        <v>314</v>
+        <v>505</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="O14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
-        <v>1418136</v>
+        <v>1416594</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4">
-        <v>505</v>
+        <v>100</v>
       </c>
       <c r="F15" s="4">
-        <v>505</v>
+        <v>100</v>
       </c>
       <c r="L15" s="4">
-        <v>505</v>
+        <v>100</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O15" s="8">
         <v>2</v>
@@ -1372,22 +1347,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
-        <v>1418424</v>
+        <v>1404448</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D16" s="4">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E16" s="4">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O16" s="8">
         <v>1</v>
@@ -1395,25 +1370,25 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
-        <v>1416594</v>
+        <v>1418054</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D17" s="4">
-        <v>100</v>
+        <v>964.51</v>
       </c>
       <c r="F17" s="4">
-        <v>100</v>
+        <v>964.51</v>
       </c>
       <c r="L17" s="4">
-        <v>100</v>
+        <v>964.51</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="O17" s="8">
         <v>2</v>
@@ -1421,22 +1396,22 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
-        <v>1404448</v>
+        <v>1414735</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="D18" s="4">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="E18" s="4">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O18" s="8">
         <v>1</v>
@@ -1444,97 +1419,109 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
-        <v>1418054</v>
+        <v>1415442</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="D19" s="4">
-        <v>964.51</v>
-      </c>
-      <c r="F19" s="4">
-        <v>964.51</v>
-      </c>
-      <c r="L19" s="4">
-        <v>964.51</v>
+        <v>505</v>
+      </c>
+      <c r="E19" s="4">
+        <v>505</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="O19" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
-        <v>1414735</v>
+        <v>1418029</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="4">
-        <v>505</v>
-      </c>
-      <c r="E20" s="4">
-        <v>505</v>
+        <v>205</v>
+      </c>
+      <c r="F20" s="4">
+        <v>205</v>
+      </c>
+      <c r="L20" s="4">
+        <v>205</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="O20" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
-        <v>1415442</v>
+        <v>1418176</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4">
-        <v>505</v>
-      </c>
-      <c r="E21" s="4">
-        <v>505</v>
+        <v>1245</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1245</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1245</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="O21" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
-        <v>1418029</v>
+        <v>1415202</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4">
-        <v>205</v>
+        <v>591.22</v>
+      </c>
+      <c r="E22" s="4">
+        <v>247.03</v>
       </c>
       <c r="F22" s="4">
-        <v>205</v>
-      </c>
-      <c r="L22" s="4">
-        <v>205</v>
+        <v>344.19</v>
+      </c>
+      <c r="G22" s="4">
+        <v>12.36</v>
+      </c>
+      <c r="H22" s="4">
+        <v>267.24</v>
+      </c>
+      <c r="I22" s="4">
+        <v>64.59</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="O22" s="8">
         <v>2</v>
@@ -1542,25 +1529,28 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
-        <v>1418176</v>
+        <v>1412075</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="D23" s="4">
-        <v>1245</v>
+        <v>1041.45</v>
+      </c>
+      <c r="E23" s="4">
+        <v>608.45000000000005</v>
       </c>
       <c r="F23" s="4">
-        <v>1245</v>
-      </c>
-      <c r="L23" s="4">
-        <v>1245</v>
+        <v>433</v>
+      </c>
+      <c r="G23" s="4">
+        <v>433</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="O23" s="8">
         <v>2</v>
@@ -1568,86 +1558,68 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
-        <v>1415202</v>
+        <v>1417652</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="D24" s="4">
-        <v>591.22</v>
+        <v>486.23</v>
       </c>
       <c r="E24" s="4">
-        <v>247.03</v>
-      </c>
-      <c r="F24" s="4">
-        <v>344.19</v>
-      </c>
-      <c r="G24" s="4">
-        <v>12.36</v>
-      </c>
-      <c r="H24" s="4">
-        <v>267.24</v>
-      </c>
-      <c r="I24" s="4">
-        <v>64.59</v>
+        <v>486.23</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="O24" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
-        <v>1412075</v>
+        <v>1410247</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D25" s="4">
-        <v>1041.45</v>
+        <v>433</v>
       </c>
       <c r="E25" s="4">
-        <v>608.45000000000005</v>
-      </c>
-      <c r="F25" s="4">
         <v>433</v>
       </c>
-      <c r="G25" s="4">
-        <v>433</v>
-      </c>
       <c r="N25" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="O25" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
-        <v>1417652</v>
+        <v>1418126</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="D26" s="4">
-        <v>486.23</v>
+        <v>433</v>
       </c>
       <c r="E26" s="4">
-        <v>486.23</v>
+        <v>433</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O26" s="8">
         <v>1</v>
@@ -1655,22 +1627,22 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
-        <v>1417701</v>
+        <v>1418043</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="D27" s="4">
-        <v>154.07</v>
+        <v>577.5</v>
       </c>
       <c r="E27" s="4">
-        <v>154.07</v>
+        <v>577.5</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O27" s="8">
         <v>1</v>
@@ -1678,109 +1650,127 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
-        <v>1410247</v>
+        <v>1415743</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4">
-        <v>433</v>
+        <v>3011.86</v>
       </c>
       <c r="E28" s="4">
-        <v>433</v>
+        <v>450</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2561.86</v>
+      </c>
+      <c r="G28" s="4">
+        <v>450</v>
+      </c>
+      <c r="H28" s="4">
+        <v>450</v>
+      </c>
+      <c r="I28" s="4">
+        <v>450</v>
+      </c>
+      <c r="J28" s="4">
+        <v>450</v>
+      </c>
+      <c r="K28" s="4">
+        <v>761.86</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="O28" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
-        <v>1418126</v>
+        <v>1417895</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D29" s="4">
-        <v>433</v>
+        <v>862</v>
       </c>
       <c r="E29" s="4">
         <v>433</v>
       </c>
+      <c r="F29" s="4">
+        <v>429</v>
+      </c>
+      <c r="G29" s="4">
+        <v>429</v>
+      </c>
       <c r="N29" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O29" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
-        <v>1418043</v>
+        <v>1415049</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="D30" s="4">
-        <v>577.5</v>
+        <v>754.5</v>
       </c>
       <c r="E30" s="4">
         <v>577.5</v>
       </c>
+      <c r="F30" s="4">
+        <v>177</v>
+      </c>
+      <c r="G30" s="4">
+        <v>177</v>
+      </c>
       <c r="N30" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O30" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
-        <v>1415743</v>
+        <v>1400549</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D31" s="4">
-        <v>3011.86</v>
+        <v>437.46</v>
       </c>
       <c r="E31" s="4">
-        <v>450</v>
+        <v>218.73</v>
       </c>
       <c r="F31" s="4">
-        <v>2561.86</v>
+        <v>218.73</v>
       </c>
       <c r="G31" s="4">
-        <v>450</v>
-      </c>
-      <c r="H31" s="4">
-        <v>450</v>
-      </c>
-      <c r="I31" s="4">
-        <v>450</v>
-      </c>
-      <c r="J31" s="4">
-        <v>450</v>
-      </c>
-      <c r="K31" s="4">
-        <v>761.86</v>
+        <v>218.73</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="O31" s="8">
         <v>2</v>
@@ -1788,28 +1778,28 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
-        <v>1417895</v>
+        <v>1413859</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="D32" s="4">
-        <v>862</v>
+        <v>343</v>
       </c>
       <c r="E32" s="4">
-        <v>433</v>
+        <v>303</v>
       </c>
       <c r="F32" s="4">
-        <v>429</v>
+        <v>40</v>
       </c>
       <c r="G32" s="4">
-        <v>429</v>
+        <v>40</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="O32" s="8">
         <v>2</v>
@@ -1817,57 +1807,51 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
-        <v>1415049</v>
+        <v>1414091</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D33" s="4">
-        <v>754.5</v>
+        <v>110.45</v>
       </c>
       <c r="E33" s="4">
-        <v>577.5</v>
-      </c>
-      <c r="F33" s="4">
-        <v>177</v>
-      </c>
-      <c r="G33" s="4">
-        <v>177</v>
+        <v>110.45</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="O33" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
-        <v>1400549</v>
+        <v>1407796</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D34" s="4">
-        <v>437.46</v>
+        <v>1106</v>
       </c>
       <c r="E34" s="4">
-        <v>218.73</v>
+        <v>553</v>
       </c>
       <c r="F34" s="4">
-        <v>218.73</v>
+        <v>553</v>
       </c>
       <c r="G34" s="4">
-        <v>218.73</v>
+        <v>553</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="O34" s="8">
         <v>2</v>
@@ -1875,28 +1859,31 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
-        <v>1413859</v>
+        <v>1416467</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D35" s="4">
-        <v>343</v>
+        <v>1056</v>
       </c>
       <c r="E35" s="4">
-        <v>303</v>
+        <v>433</v>
       </c>
       <c r="F35" s="4">
-        <v>40</v>
+        <v>623</v>
       </c>
       <c r="G35" s="4">
-        <v>40</v>
+        <v>190</v>
+      </c>
+      <c r="H35" s="4">
+        <v>433</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="O35" s="8">
         <v>2</v>
@@ -1904,22 +1891,22 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
-        <v>1414091</v>
+        <v>1418387</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="D36" s="4">
-        <v>110.45</v>
+        <v>216.88</v>
       </c>
       <c r="E36" s="4">
-        <v>110.45</v>
+        <v>216.88</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O36" s="8">
         <v>1</v>
@@ -1927,28 +1914,25 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
-        <v>1407796</v>
+        <v>1418336</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D37" s="4">
-        <v>1106</v>
-      </c>
-      <c r="E37" s="4">
-        <v>553</v>
+        <v>157.47999999999999</v>
       </c>
       <c r="F37" s="4">
-        <v>553</v>
-      </c>
-      <c r="G37" s="4">
-        <v>553</v>
+        <v>157.47999999999999</v>
+      </c>
+      <c r="J37" s="4">
+        <v>157.47999999999999</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="O37" s="8">
         <v>2</v>
@@ -1956,54 +1940,45 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
-        <v>1416467</v>
+        <v>1413119</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="D38" s="4">
-        <v>1056</v>
+        <v>64</v>
       </c>
       <c r="E38" s="4">
-        <v>433</v>
-      </c>
-      <c r="F38" s="4">
-        <v>623</v>
-      </c>
-      <c r="G38" s="4">
-        <v>190</v>
-      </c>
-      <c r="H38" s="4">
-        <v>433</v>
+        <v>64</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="O38" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
-        <v>1418387</v>
+        <v>1411108</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="D39" s="4">
-        <v>216.88</v>
+        <v>72.180000000000007</v>
       </c>
       <c r="E39" s="4">
-        <v>216.88</v>
+        <v>72.180000000000007</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O39" s="8">
         <v>1</v>
@@ -2011,25 +1986,43 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
-        <v>1418336</v>
+        <v>1418213</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="D40" s="4">
-        <v>157.47999999999999</v>
+        <v>2463.09</v>
+      </c>
+      <c r="E40" s="4">
+        <v>243.33</v>
       </c>
       <c r="F40" s="4">
-        <v>157.47999999999999</v>
+        <v>2219.7600000000002</v>
+      </c>
+      <c r="G40" s="4">
+        <v>252.61</v>
+      </c>
+      <c r="H40" s="4">
+        <v>244.48</v>
+      </c>
+      <c r="I40" s="4">
+        <v>473.47</v>
       </c>
       <c r="J40" s="4">
-        <v>157.47999999999999</v>
+        <v>248.89</v>
+      </c>
+      <c r="K40" s="4">
+        <v>257.08999999999997</v>
+      </c>
+      <c r="L40" s="4">
+        <v>743.22</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="O40" s="8">
         <v>2</v>
@@ -2037,22 +2030,22 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
-        <v>1413119</v>
+        <v>1412543</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="D41" s="4">
-        <v>64</v>
+        <v>472.45</v>
       </c>
       <c r="E41" s="4">
-        <v>64</v>
+        <v>472.45</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O41" s="8">
         <v>1</v>
@@ -2060,22 +2053,22 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
-        <v>1411108</v>
+        <v>1418401</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D42" s="4">
-        <v>72.180000000000007</v>
+        <v>214.05</v>
       </c>
       <c r="E42" s="4">
-        <v>72.180000000000007</v>
+        <v>214.05</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O42" s="8">
         <v>1</v>
@@ -2083,66 +2076,45 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
-        <v>1418213</v>
+        <v>1417186</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D43" s="4">
-        <v>2463.09</v>
+        <v>227.98</v>
       </c>
       <c r="E43" s="4">
-        <v>243.33</v>
-      </c>
-      <c r="F43" s="4">
-        <v>2219.7600000000002</v>
-      </c>
-      <c r="G43" s="4">
-        <v>252.61</v>
-      </c>
-      <c r="H43" s="4">
-        <v>244.48</v>
-      </c>
-      <c r="I43" s="4">
-        <v>473.47</v>
-      </c>
-      <c r="J43" s="4">
-        <v>248.89</v>
-      </c>
-      <c r="K43" s="4">
-        <v>257.08999999999997</v>
-      </c>
-      <c r="L43" s="4">
-        <v>743.22</v>
+        <v>227.98</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="O43" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
-        <v>1412543</v>
+        <v>1418470</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D44" s="4">
-        <v>472.45</v>
+        <v>210.11</v>
       </c>
       <c r="E44" s="4">
-        <v>472.45</v>
+        <v>210.11</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O44" s="8">
         <v>1</v>
@@ -2150,22 +2122,22 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
-        <v>1418401</v>
+        <v>1410278</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>144</v>
+        <v>25</v>
       </c>
       <c r="D45" s="4">
-        <v>214.05</v>
+        <v>217.78</v>
       </c>
       <c r="E45" s="4">
-        <v>214.05</v>
+        <v>217.78</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O45" s="8">
         <v>1</v>
@@ -2173,45 +2145,48 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
-        <v>1417186</v>
+        <v>1410023</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D46" s="4">
-        <v>227.98</v>
-      </c>
-      <c r="E46" s="4">
-        <v>227.98</v>
+        <v>485.08</v>
+      </c>
+      <c r="F46" s="4">
+        <v>485.08</v>
+      </c>
+      <c r="L46" s="4">
+        <v>485.08</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="O46" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
-        <v>1418470</v>
+        <v>1418267</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D47" s="4">
-        <v>210.11</v>
+        <v>220.32</v>
       </c>
       <c r="E47" s="4">
-        <v>210.11</v>
+        <v>220.32</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O47" s="8">
         <v>1</v>
@@ -2219,48 +2194,60 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
-        <v>1410278</v>
+        <v>1411226</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D48" s="4">
-        <v>217.78</v>
-      </c>
-      <c r="E48" s="4">
-        <v>217.78</v>
+        <v>879.77</v>
+      </c>
+      <c r="F48" s="4">
+        <v>879.77</v>
+      </c>
+      <c r="J48" s="4">
+        <v>210.8</v>
+      </c>
+      <c r="K48" s="4">
+        <v>221.97</v>
+      </c>
+      <c r="L48" s="4">
+        <v>447</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="O48" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
-        <v>1410023</v>
+        <v>1418416</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="D49" s="4">
-        <v>485.08</v>
+        <v>399.54</v>
+      </c>
+      <c r="E49" s="4">
+        <v>199.19</v>
       </c>
       <c r="F49" s="4">
-        <v>485.08</v>
-      </c>
-      <c r="L49" s="4">
-        <v>485.08</v>
+        <v>200.35</v>
+      </c>
+      <c r="G49" s="4">
+        <v>200.35</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="O49" s="8">
         <v>2</v>
@@ -2268,22 +2255,22 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
-        <v>1418267</v>
+        <v>1418395</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="D50" s="4">
-        <v>220.32</v>
+        <v>163</v>
       </c>
       <c r="E50" s="4">
-        <v>220.32</v>
+        <v>163</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O50" s="8">
         <v>1</v>
@@ -2291,60 +2278,51 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
-        <v>1411226</v>
+        <v>1418334</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D51" s="4">
-        <v>879.77</v>
-      </c>
-      <c r="F51" s="4">
-        <v>879.77</v>
-      </c>
-      <c r="J51" s="4">
-        <v>210.8</v>
-      </c>
-      <c r="K51" s="4">
-        <v>221.97</v>
-      </c>
-      <c r="L51" s="4">
-        <v>447</v>
+        <v>237.5</v>
+      </c>
+      <c r="E51" s="4">
+        <v>237.5</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="O51" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
-        <v>1418416</v>
+        <v>1418355</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="D52" s="4">
-        <v>399.54</v>
+        <v>544.97</v>
       </c>
       <c r="E52" s="4">
-        <v>199.19</v>
+        <v>263.97000000000003</v>
       </c>
       <c r="F52" s="4">
-        <v>200.35</v>
+        <v>281</v>
       </c>
       <c r="G52" s="4">
-        <v>200.35</v>
+        <v>281</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="O52" s="8">
         <v>2</v>
@@ -2352,22 +2330,22 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
-        <v>1418395</v>
+        <v>1412845</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D53" s="4">
-        <v>163</v>
+        <v>575</v>
       </c>
       <c r="E53" s="4">
-        <v>163</v>
+        <v>575</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O53" s="8">
         <v>1</v>
@@ -2375,22 +2353,22 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
-        <v>1416470</v>
+        <v>1418360</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D54" s="4">
-        <v>217.9</v>
+        <v>492.5</v>
       </c>
       <c r="E54" s="4">
-        <v>217.9</v>
+        <v>492.5</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O54" s="8">
         <v>1</v>
@@ -2398,22 +2376,22 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
-        <v>1418334</v>
+        <v>1417961</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="D55" s="4">
-        <v>237.5</v>
+        <v>575</v>
       </c>
       <c r="E55" s="4">
-        <v>237.5</v>
+        <v>575</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O55" s="8">
         <v>1</v>
@@ -2421,51 +2399,45 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
-        <v>1418355</v>
+        <v>1405323</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="D56" s="4">
-        <v>544.97</v>
+        <v>675</v>
       </c>
       <c r="E56" s="4">
-        <v>263.97000000000003</v>
-      </c>
-      <c r="F56" s="4">
-        <v>281</v>
-      </c>
-      <c r="G56" s="4">
-        <v>281</v>
+        <v>675</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="O56" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
-        <v>1412845</v>
+        <v>1417215</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="D57" s="4">
-        <v>575</v>
+        <v>675</v>
       </c>
       <c r="E57" s="4">
-        <v>575</v>
+        <v>675</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="O57" s="8">
         <v>1</v>
@@ -2473,68 +2445,68 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
-        <v>1418360</v>
+        <v>1415907</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="D58" s="4">
-        <v>492.5</v>
+        <v>1350</v>
       </c>
       <c r="E58" s="4">
-        <v>492.5</v>
+        <v>675</v>
+      </c>
+      <c r="F58" s="4">
+        <v>675</v>
+      </c>
+      <c r="G58" s="4">
+        <v>675</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O58" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
-        <v>1417961</v>
+        <v>1413700</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="D59" s="4">
-        <v>575</v>
+        <v>6842.04</v>
       </c>
       <c r="E59" s="4">
-        <v>575</v>
-      </c>
-      <c r="N59" s="4" t="s">
-        <v>120</v>
+        <v>6842.04</v>
+      </c>
+      <c r="N59" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="O59" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
-        <v>1405323</v>
+        <v>1415424</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="D60" s="4">
-        <v>675</v>
+        <v>2803.96</v>
       </c>
       <c r="E60" s="4">
-        <v>675</v>
-      </c>
-      <c r="N60" s="4" t="s">
-        <v>120</v>
+        <v>2803.96</v>
+      </c>
+      <c r="N60" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="O60" s="8">
         <v>1</v>
@@ -2542,154 +2514,62 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
-        <v>1417215</v>
+        <v>1418356</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
       <c r="D61" s="4">
-        <v>675</v>
-      </c>
-      <c r="E61" s="4">
-        <v>675</v>
-      </c>
-      <c r="N61" s="4" t="s">
-        <v>120</v>
+        <v>1900</v>
+      </c>
+      <c r="F61" s="4">
+        <v>1900</v>
+      </c>
+      <c r="L61" s="4">
+        <v>1900</v>
+      </c>
+      <c r="N61" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="O61" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
-        <v>1415907</v>
+        <v>1416572</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D62" s="4">
-        <v>1350</v>
+        <v>1508.26</v>
       </c>
       <c r="E62" s="4">
-        <v>675</v>
+        <v>664.95</v>
       </c>
       <c r="F62" s="4">
-        <v>675</v>
+        <v>843.31</v>
       </c>
       <c r="G62" s="4">
-        <v>675</v>
+        <v>658.22</v>
+      </c>
+      <c r="H62" s="4">
+        <v>185.09</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="O62" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="8">
-        <v>1413700</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D63" s="4">
-        <v>6842.04</v>
-      </c>
-      <c r="E63" s="4">
-        <v>6842.04</v>
-      </c>
-      <c r="N63" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="O63" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="8">
-        <v>1415424</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D64" s="4">
-        <v>2803.96</v>
-      </c>
-      <c r="E64" s="4">
-        <v>2803.96</v>
-      </c>
-      <c r="N64" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="O64" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="8">
-        <v>1418356</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" s="4">
-        <v>1900</v>
-      </c>
-      <c r="F65" s="4">
-        <v>1900</v>
-      </c>
-      <c r="L65" s="4">
-        <v>1900</v>
-      </c>
-      <c r="N65" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O65" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="8">
-        <v>1416572</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D66" s="4">
-        <v>1508.26</v>
-      </c>
-      <c r="E66" s="4">
-        <v>664.95</v>
-      </c>
-      <c r="F66" s="4">
-        <v>843.31</v>
-      </c>
-      <c r="G66" s="4">
-        <v>658.22</v>
-      </c>
-      <c r="H66" s="4">
-        <v>185.09</v>
-      </c>
-      <c r="N66" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="O66" s="8">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O33">
-    <sortCondition ref="B3:B33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O30">
+    <sortCondition ref="B3:B30"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="M1:M2"/>

</xml_diff>